<commit_message>
now I am really confused if that's the proper version?
</commit_message>
<xml_diff>
--- a/wideband-F103/export/rev3/wideband_controller_bom.xlsx
+++ b/wideband-F103/export/rev3/wideband_controller_bom.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\wideband-F103\export\rev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Текстовый документ" sheetId="1" r:id="rId1"/>
@@ -243,9 +243,6 @@
     <t>C81598</t>
   </si>
   <si>
-    <t>BZX84C5V1LT1G</t>
-  </si>
-  <si>
     <t>D7</t>
   </si>
   <si>
@@ -744,9 +741,6 @@
     <t>Crystal:Crystal_SMD_HC49-SD</t>
   </si>
   <si>
-    <t>C47075</t>
-  </si>
-  <si>
     <t>C210835</t>
   </si>
   <si>
@@ -757,6 +751,12 @@
   </si>
   <si>
     <t>C252310</t>
+  </si>
+  <si>
+    <t>C2903789</t>
+  </si>
+  <si>
+    <t>BAT54S</t>
   </si>
 </sst>
 </file>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,1073 +2171,1073 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>75</v>
       </c>
-      <c r="C42" t="s">
-        <v>76</v>
-      </c>
       <c r="D42" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
         <v>77</v>
-      </c>
-      <c r="B43" t="s">
-        <v>78</v>
       </c>
       <c r="C43" t="s">
         <v>57</v>
       </c>
       <c r="D43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
         <v>83</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>84</v>
       </c>
-      <c r="C47" t="s">
-        <v>85</v>
-      </c>
       <c r="D47" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>87</v>
-      </c>
-      <c r="C48" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
         <v>89</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>90</v>
-      </c>
-      <c r="C49" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>93</v>
-      </c>
-      <c r="C50" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
         <v>95</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>96</v>
-      </c>
-      <c r="C51" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
         <v>98</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>99</v>
-      </c>
-      <c r="C52" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
         <v>101</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>103</v>
-      </c>
-      <c r="D53" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
         <v>105</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>106</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>107</v>
-      </c>
-      <c r="D54" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
         <v>109</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" t="s">
         <v>110</v>
-      </c>
-      <c r="C55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
         <v>114</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>115</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>116</v>
-      </c>
-      <c r="D58" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" t="s">
         <v>107</v>
-      </c>
-      <c r="D60" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" t="s">
         <v>120</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>121</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>122</v>
-      </c>
-      <c r="D61" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
         <v>124</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" t="s">
         <v>125</v>
-      </c>
-      <c r="C62" t="s">
-        <v>122</v>
-      </c>
-      <c r="D62" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C63" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" t="s">
         <v>122</v>
-      </c>
-      <c r="D63" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" t="s">
         <v>128</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" t="s">
         <v>129</v>
-      </c>
-      <c r="C64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" t="s">
         <v>132</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" t="s">
         <v>133</v>
-      </c>
-      <c r="C66" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
         <v>135</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" t="s">
         <v>136</v>
-      </c>
-      <c r="C67" t="s">
-        <v>107</v>
-      </c>
-      <c r="D67" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
         <v>139</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69" t="s">
         <v>140</v>
-      </c>
-      <c r="C69" t="s">
-        <v>107</v>
-      </c>
-      <c r="D69" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
         <v>143</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" t="s">
         <v>144</v>
-      </c>
-      <c r="C71" t="s">
-        <v>122</v>
-      </c>
-      <c r="D71" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" t="s">
         <v>146</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>147</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>148</v>
-      </c>
-      <c r="D72" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" t="s">
         <v>152</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75" t="s">
         <v>153</v>
-      </c>
-      <c r="C75" t="s">
-        <v>107</v>
-      </c>
-      <c r="D75" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C76" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" t="s">
         <v>122</v>
-      </c>
-      <c r="D76" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" t="s">
         <v>156</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" t="s">
         <v>157</v>
-      </c>
-      <c r="C77" t="s">
-        <v>107</v>
-      </c>
-      <c r="D77" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" t="s">
         <v>122</v>
-      </c>
-      <c r="D79" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C80" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D80" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C82" t="s">
+        <v>121</v>
+      </c>
+      <c r="D82" t="s">
         <v>122</v>
-      </c>
-      <c r="D82" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C83" t="s">
+        <v>121</v>
+      </c>
+      <c r="D83" t="s">
         <v>122</v>
-      </c>
-      <c r="D83" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>164</v>
+      </c>
+      <c r="B84" t="s">
         <v>165</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>106</v>
+      </c>
+      <c r="D84" t="s">
         <v>166</v>
-      </c>
-      <c r="C84" t="s">
-        <v>107</v>
-      </c>
-      <c r="D84" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" t="s">
         <v>168</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85" t="s">
         <v>169</v>
-      </c>
-      <c r="C85" t="s">
-        <v>107</v>
-      </c>
-      <c r="D85" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" t="s">
         <v>173</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
+        <v>121</v>
+      </c>
+      <c r="D88" t="s">
         <v>174</v>
-      </c>
-      <c r="C88" t="s">
-        <v>122</v>
-      </c>
-      <c r="D88" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>176</v>
+      </c>
+      <c r="B90" t="s">
         <v>177</v>
       </c>
-      <c r="B90" t="s">
-        <v>178</v>
-      </c>
       <c r="C90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D91" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>179</v>
+      </c>
+      <c r="B92" t="s">
         <v>180</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" t="s">
         <v>181</v>
-      </c>
-      <c r="C92" t="s">
-        <v>122</v>
-      </c>
-      <c r="D92" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>183</v>
+      </c>
+      <c r="B94" t="s">
         <v>184</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" t="s">
         <v>185</v>
-      </c>
-      <c r="C94" t="s">
-        <v>107</v>
-      </c>
-      <c r="D94" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D95" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C96" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C97" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C98" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" t="s">
         <v>191</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" t="s">
         <v>192</v>
-      </c>
-      <c r="C99" t="s">
-        <v>107</v>
-      </c>
-      <c r="D99" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D100" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C101" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D102" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C103" t="s">
+        <v>121</v>
+      </c>
+      <c r="D103" t="s">
         <v>122</v>
-      </c>
-      <c r="D103" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C104" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D104" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C105" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D105" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B106" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D106" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>200</v>
+      </c>
+      <c r="B107" t="s">
         <v>201</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>202</v>
-      </c>
-      <c r="C107" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>204</v>
+      </c>
+      <c r="B109" t="s">
         <v>205</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>206</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>207</v>
-      </c>
-      <c r="D109" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" t="s">
         <v>209</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>210</v>
       </c>
-      <c r="C110" t="s">
-        <v>211</v>
-      </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>211</v>
+      </c>
+      <c r="B111" t="s">
         <v>212</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>213</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>214</v>
-      </c>
-      <c r="D111" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" t="s">
         <v>216</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
+        <v>102</v>
+      </c>
+      <c r="D112" t="s">
         <v>217</v>
-      </c>
-      <c r="C112" t="s">
-        <v>103</v>
-      </c>
-      <c r="D112" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>218</v>
+      </c>
+      <c r="B113" t="s">
         <v>219</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
+        <v>75</v>
+      </c>
+      <c r="D113" t="s">
         <v>220</v>
-      </c>
-      <c r="C113" t="s">
-        <v>76</v>
-      </c>
-      <c r="D113" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" t="s">
         <v>222</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
+        <v>75</v>
+      </c>
+      <c r="D114" t="s">
         <v>223</v>
-      </c>
-      <c r="C114" t="s">
-        <v>76</v>
-      </c>
-      <c r="D114" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>224</v>
+      </c>
+      <c r="B115" t="s">
         <v>225</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>226</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>227</v>
-      </c>
-      <c r="D115" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>228</v>
+      </c>
+      <c r="B116" t="s">
         <v>229</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>230</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>231</v>
-      </c>
-      <c r="D116" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" t="s">
         <v>233</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>234</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>235</v>
-      </c>
-      <c r="D117" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B118" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C118" t="s">
+        <v>234</v>
+      </c>
+      <c r="D118" t="s">
         <v>235</v>
-      </c>
-      <c r="D118" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" t="s">
         <v>238</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>239</v>
       </c>
-      <c r="C119" t="s">
-        <v>240</v>
-      </c>
       <c r="D119" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>